<commit_message>
Adapt references in raw dataset
Some references were interpreted by R as dates. This was corrected in the raw dataset
</commit_message>
<xml_diff>
--- a/data/raw/copy_of_10530_2016_1278_MOESM2_ESM.xlsx
+++ b/data/raw/copy_of_10530_2016_1278_MOESM2_ESM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3592" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3595" uniqueCount="615">
   <si>
     <t>Environment</t>
   </si>
@@ -5927,6 +5927,15 @@
   </si>
   <si>
     <t>higher_classification</t>
+  </si>
+  <si>
+    <t>1-3</t>
+  </si>
+  <si>
+    <t>1-9</t>
+  </si>
+  <si>
+    <t>1-12</t>
   </si>
 </sst>
 </file>
@@ -6123,9 +6132,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -6205,6 +6211,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6510,8 +6519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V360"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
-      <selection activeCell="A240" sqref="A240:XFD240"/>
+    <sheetView tabSelected="1" topLeftCell="A352" workbookViewId="0">
+      <selection activeCell="V271" sqref="V271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6526,61 +6535,61 @@
       <c r="A1" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>611</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>587</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>588</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="23" t="s">
         <v>589</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="25" t="s">
         <v>590</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="24" t="s">
         <v>591</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>592</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="23" t="s">
         <v>593</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="25" t="s">
         <v>594</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>595</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="24" t="s">
         <v>596</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="M1" s="23" t="s">
         <v>597</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="N1" s="23" t="s">
         <v>598</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="25" t="s">
         <v>599</v>
       </c>
-      <c r="P1" s="25" t="s">
+      <c r="P1" s="24" t="s">
         <v>600</v>
       </c>
-      <c r="Q1" s="24" t="s">
+      <c r="Q1" s="23" t="s">
         <v>601</v>
       </c>
-      <c r="R1" s="24" t="s">
+      <c r="R1" s="23" t="s">
         <v>602</v>
       </c>
-      <c r="S1" s="24" t="s">
+      <c r="S1" s="23" t="s">
         <v>603</v>
       </c>
-      <c r="T1" s="26" t="s">
+      <c r="T1" s="25" t="s">
         <v>604</v>
       </c>
       <c r="U1" s="1" t="s">
@@ -6594,7 +6603,7 @@
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C2" s="4"/>
@@ -6632,15 +6641,15 @@
       <c r="U2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="8">
-        <v>43160</v>
+      <c r="V2" s="35" t="s">
+        <v>612</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C3" s="4"/>
@@ -6684,7 +6693,7 @@
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C4" s="4"/>
@@ -6730,7 +6739,7 @@
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -6784,7 +6793,7 @@
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -6831,10 +6840,10 @@
       </c>
     </row>
     <row r="7" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -6884,15 +6893,15 @@
       <c r="U7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="V7" s="8">
-        <v>43344</v>
+      <c r="V7" s="35" t="s">
+        <v>613</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -6944,7 +6953,7 @@
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -7004,7 +7013,7 @@
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -7060,7 +7069,7 @@
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -7114,7 +7123,7 @@
       <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -7164,7 +7173,7 @@
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -7220,7 +7229,7 @@
       <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -7276,7 +7285,7 @@
       <c r="A15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -7330,7 +7339,7 @@
       <c r="A16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -7388,7 +7397,7 @@
       <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -7442,7 +7451,7 @@
       <c r="A18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -7496,7 +7505,7 @@
       <c r="A19" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C19" s="4"/>
@@ -7536,7 +7545,7 @@
       <c r="A20" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -7592,7 +7601,7 @@
       <c r="A21" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -7650,7 +7659,7 @@
       <c r="A22" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -7706,7 +7715,7 @@
       <c r="A23" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -7756,15 +7765,15 @@
       <c r="U23" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="V23" s="8">
-        <v>43435</v>
+      <c r="V23" s="35" t="s">
+        <v>614</v>
       </c>
     </row>
     <row r="24" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C24" s="4"/>
@@ -7814,7 +7823,7 @@
       <c r="A25" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -7872,7 +7881,7 @@
       <c r="A26" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -7930,7 +7939,7 @@
       <c r="A27" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -7978,7 +7987,7 @@
       <c r="A28" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -8038,7 +8047,7 @@
       <c r="A29" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -8096,7 +8105,7 @@
       <c r="A30" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -8150,7 +8159,7 @@
       <c r="A31" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="34" t="s">
+      <c r="B31" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -8198,7 +8207,7 @@
       <c r="A32" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -8258,7 +8267,7 @@
       <c r="A33" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="34" t="s">
+      <c r="B33" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C33" s="4" t="s">
@@ -8316,7 +8325,7 @@
       <c r="A34" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="34" t="s">
+      <c r="B34" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -8372,7 +8381,7 @@
       <c r="A35" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="34" t="s">
+      <c r="B35" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C35" s="4" t="s">
@@ -8424,7 +8433,7 @@
       <c r="A36" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="34" t="s">
+      <c r="B36" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C36" s="4"/>
@@ -8468,7 +8477,7 @@
       <c r="A37" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B37" s="34" t="s">
+      <c r="B37" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C37" s="4" t="s">
@@ -8512,7 +8521,7 @@
       <c r="A38" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B38" s="34" t="s">
+      <c r="B38" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C38" s="4" t="s">
@@ -8570,7 +8579,7 @@
       <c r="A39" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B39" s="34" t="s">
+      <c r="B39" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C39" s="4" t="s">
@@ -8626,7 +8635,7 @@
       <c r="A40" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B40" s="34" t="s">
+      <c r="B40" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -8664,7 +8673,7 @@
       <c r="A41" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B41" s="34" t="s">
+      <c r="B41" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C41" s="4" t="s">
@@ -8722,7 +8731,7 @@
       <c r="A42" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B42" s="34" t="s">
+      <c r="B42" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C42" s="4" t="s">
@@ -8778,7 +8787,7 @@
       <c r="A43" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B43" s="34" t="s">
+      <c r="B43" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C43" s="4" t="s">
@@ -8826,7 +8835,7 @@
       <c r="A44" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B44" s="34" t="s">
+      <c r="B44" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -8884,7 +8893,7 @@
       <c r="A45" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B45" s="34" t="s">
+      <c r="B45" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C45" s="4" t="s">
@@ -8940,7 +8949,7 @@
       <c r="A46" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B46" s="34" t="s">
+      <c r="B46" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C46" s="4" t="s">
@@ -8996,7 +9005,7 @@
       <c r="A47" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B47" s="34" t="s">
+      <c r="B47" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C47" s="4" t="s">
@@ -9052,7 +9061,7 @@
       <c r="A48" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B48" s="34" t="s">
+      <c r="B48" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C48" s="4" t="s">
@@ -9108,7 +9117,7 @@
       <c r="A49" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B49" s="34" t="s">
+      <c r="B49" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C49" s="4" t="s">
@@ -9164,7 +9173,7 @@
       <c r="A50" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B50" s="34" t="s">
+      <c r="B50" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C50" s="4" t="s">
@@ -9224,7 +9233,7 @@
       <c r="A51" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B51" s="34" t="s">
+      <c r="B51" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C51" s="4" t="s">
@@ -9280,7 +9289,7 @@
       <c r="A52" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="34" t="s">
+      <c r="B52" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C52" s="4" t="s">
@@ -9340,7 +9349,7 @@
       <c r="A53" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B53" s="34" t="s">
+      <c r="B53" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C53" s="4" t="s">
@@ -9400,7 +9409,7 @@
       <c r="A54" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B54" s="34" t="s">
+      <c r="B54" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C54" s="4" t="s">
@@ -9448,7 +9457,7 @@
       <c r="A55" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B55" s="34" t="s">
+      <c r="B55" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C55" s="4"/>
@@ -9496,7 +9505,7 @@
       <c r="A56" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B56" s="34" t="s">
+      <c r="B56" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C56" s="4"/>
@@ -9534,7 +9543,7 @@
       <c r="A57" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B57" s="34" t="s">
+      <c r="B57" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C57" s="4" t="s">
@@ -9588,7 +9597,7 @@
       <c r="A58" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B58" s="34" t="s">
+      <c r="B58" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C58" s="4" t="s">
@@ -9638,7 +9647,7 @@
       <c r="A59" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B59" s="34" t="s">
+      <c r="B59" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C59" s="4" t="s">
@@ -9688,7 +9697,7 @@
       <c r="A60" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B60" s="34" t="s">
+      <c r="B60" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C60" s="4" t="s">
@@ -9742,7 +9751,7 @@
       <c r="A61" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B61" s="34" t="s">
+      <c r="B61" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C61" s="4" t="s">
@@ -9800,7 +9809,7 @@
       <c r="A62" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B62" s="34" t="s">
+      <c r="B62" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C62" s="4" t="s">
@@ -9842,7 +9851,7 @@
       <c r="A63" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B63" s="34" t="s">
+      <c r="B63" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C63" s="4" t="s">
@@ -9898,7 +9907,7 @@
       <c r="A64" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B64" s="34" t="s">
+      <c r="B64" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C64" s="4" t="s">
@@ -9954,7 +9963,7 @@
       <c r="A65" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B65" s="34" t="s">
+      <c r="B65" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C65" s="6" t="s">
@@ -10010,7 +10019,7 @@
       <c r="A66" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B66" s="34" t="s">
+      <c r="B66" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C66" s="6" t="s">
@@ -10062,7 +10071,7 @@
       <c r="A67" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B67" s="34" t="s">
+      <c r="B67" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C67" s="6" t="s">
@@ -10110,7 +10119,7 @@
       <c r="A68" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B68" s="34" t="s">
+      <c r="B68" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C68" s="6" t="s">
@@ -10158,7 +10167,7 @@
       <c r="A69" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B69" s="34" t="s">
+      <c r="B69" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C69" s="6" t="s">
@@ -10214,7 +10223,7 @@
       <c r="A70" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B70" s="34" t="s">
+      <c r="B70" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C70" s="6" t="s">
@@ -10268,7 +10277,7 @@
       <c r="A71" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B71" s="34" t="s">
+      <c r="B71" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C71" s="6" t="s">
@@ -10326,7 +10335,7 @@
       <c r="A72" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B72" s="34" t="s">
+      <c r="B72" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C72" s="6" t="s">
@@ -10384,7 +10393,7 @@
       <c r="A73" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B73" s="34" t="s">
+      <c r="B73" s="33" t="s">
         <v>606</v>
       </c>
       <c r="C73" s="6" t="s">
@@ -10435,64 +10444,64 @@
       </c>
     </row>
     <row r="74" spans="1:22" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="10" t="s">
+      <c r="A74" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B74" s="34" t="s">
+      <c r="B74" s="33" t="s">
         <v>606</v>
       </c>
-      <c r="C74" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D74" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E74" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F74" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="G74" s="11">
+      <c r="C74" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D74" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F74" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G74" s="10">
         <v>1800</v>
       </c>
-      <c r="H74" s="11">
+      <c r="H74" s="10">
         <v>1800</v>
       </c>
-      <c r="I74" s="11">
+      <c r="I74" s="10">
         <v>1835</v>
       </c>
-      <c r="J74" s="12">
+      <c r="J74" s="11">
         <v>1900</v>
       </c>
-      <c r="K74" s="12" t="s">
+      <c r="K74" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="L74" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="M74" s="11"/>
-      <c r="N74" s="11"/>
-      <c r="O74" s="12"/>
-      <c r="P74" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q74" s="11"/>
-      <c r="R74" s="11"/>
-      <c r="S74" s="11"/>
-      <c r="T74" s="12"/>
-      <c r="U74" s="12" t="s">
+      <c r="L74" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M74" s="10"/>
+      <c r="N74" s="10"/>
+      <c r="O74" s="11"/>
+      <c r="P74" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q74" s="10"/>
+      <c r="R74" s="10"/>
+      <c r="S74" s="10"/>
+      <c r="T74" s="11"/>
+      <c r="U74" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="V74" s="11" t="s">
+      <c r="V74" s="10" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="75" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A75" s="9" t="s">
+      <c r="A75" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="B75" s="35" t="s">
+      <c r="B75" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C75" s="6"/>
@@ -10531,10 +10540,10 @@
       </c>
     </row>
     <row r="76" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A76" s="9" t="s">
+      <c r="A76" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B76" s="35" t="s">
+      <c r="B76" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C76" s="6"/>
@@ -10573,10 +10582,10 @@
       </c>
     </row>
     <row r="77" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="9" t="s">
+      <c r="A77" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="B77" s="35" t="s">
+      <c r="B77" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C77" s="6" t="s">
@@ -10611,10 +10620,10 @@
       </c>
     </row>
     <row r="78" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A78" s="9" t="s">
+      <c r="A78" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="B78" s="35" t="s">
+      <c r="B78" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C78" s="6" t="s">
@@ -10665,10 +10674,10 @@
       </c>
     </row>
     <row r="79" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="9" t="s">
+      <c r="A79" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="B79" s="35" t="s">
+      <c r="B79" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C79" s="6" t="s">
@@ -10705,10 +10714,10 @@
       </c>
     </row>
     <row r="80" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="9" t="s">
+      <c r="A80" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B80" s="35" t="s">
+      <c r="B80" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C80" s="6" t="s">
@@ -10745,10 +10754,10 @@
       </c>
     </row>
     <row r="81" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A81" s="9" t="s">
+      <c r="A81" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B81" s="35" t="s">
+      <c r="B81" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C81" s="6"/>
@@ -10789,10 +10798,10 @@
       </c>
     </row>
     <row r="82" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A82" s="9" t="s">
+      <c r="A82" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="B82" s="35" t="s">
+      <c r="B82" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C82" s="6" t="s">
@@ -10839,10 +10848,10 @@
       </c>
     </row>
     <row r="83" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A83" s="9" t="s">
+      <c r="A83" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="B83" s="35" t="s">
+      <c r="B83" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C83" s="6" t="s">
@@ -10879,10 +10888,10 @@
       </c>
     </row>
     <row r="84" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A84" s="9" t="s">
+      <c r="A84" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="B84" s="35" t="s">
+      <c r="B84" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C84" s="6"/>
@@ -10921,10 +10930,10 @@
       </c>
     </row>
     <row r="85" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A85" s="9" t="s">
+      <c r="A85" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="B85" s="35" t="s">
+      <c r="B85" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C85" s="6"/>
@@ -10961,10 +10970,10 @@
       </c>
     </row>
     <row r="86" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A86" s="9" t="s">
+      <c r="A86" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="B86" s="35" t="s">
+      <c r="B86" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C86" s="6" t="s">
@@ -11005,10 +11014,10 @@
       </c>
     </row>
     <row r="87" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A87" s="9" t="s">
+      <c r="A87" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="B87" s="35" t="s">
+      <c r="B87" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C87" s="6" t="s">
@@ -11043,10 +11052,10 @@
       </c>
     </row>
     <row r="88" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A88" s="9" t="s">
+      <c r="A88" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="B88" s="35" t="s">
+      <c r="B88" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C88" s="6"/>
@@ -11085,10 +11094,10 @@
       </c>
     </row>
     <row r="89" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A89" s="9" t="s">
+      <c r="A89" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="B89" s="35" t="s">
+      <c r="B89" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C89" s="6" t="s">
@@ -11133,10 +11142,10 @@
       </c>
     </row>
     <row r="90" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A90" s="9" t="s">
+      <c r="A90" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="B90" s="35" t="s">
+      <c r="B90" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C90" s="6" t="s">
@@ -11171,10 +11180,10 @@
       </c>
     </row>
     <row r="91" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A91" s="9" t="s">
+      <c r="A91" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="B91" s="35" t="s">
+      <c r="B91" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C91" s="6" t="s">
@@ -11209,10 +11218,10 @@
       </c>
     </row>
     <row r="92" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A92" s="9" t="s">
+      <c r="A92" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="B92" s="35" t="s">
+      <c r="B92" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C92" s="6" t="s">
@@ -11257,10 +11266,10 @@
       </c>
     </row>
     <row r="93" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="9" t="s">
+      <c r="A93" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="B93" s="35" t="s">
+      <c r="B93" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C93" s="6"/>
@@ -11301,10 +11310,10 @@
       </c>
     </row>
     <row r="94" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A94" s="9" t="s">
+      <c r="A94" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="B94" s="35" t="s">
+      <c r="B94" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C94" s="6"/>
@@ -11349,10 +11358,10 @@
       </c>
     </row>
     <row r="95" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A95" s="9" t="s">
+      <c r="A95" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="B95" s="35" t="s">
+      <c r="B95" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C95" s="6" t="s">
@@ -11401,10 +11410,10 @@
       </c>
     </row>
     <row r="96" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A96" s="9" t="s">
+      <c r="A96" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="B96" s="35" t="s">
+      <c r="B96" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C96" s="6" t="s">
@@ -11441,10 +11450,10 @@
       </c>
     </row>
     <row r="97" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A97" s="9" t="s">
+      <c r="A97" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="B97" s="35" t="s">
+      <c r="B97" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C97" s="6" t="s">
@@ -11499,10 +11508,10 @@
       </c>
     </row>
     <row r="98" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A98" s="9" t="s">
+      <c r="A98" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="B98" s="35" t="s">
+      <c r="B98" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C98" s="6" t="s">
@@ -11549,10 +11558,10 @@
       </c>
     </row>
     <row r="99" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A99" s="9" t="s">
+      <c r="A99" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="B99" s="35" t="s">
+      <c r="B99" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C99" s="6"/>
@@ -11593,10 +11602,10 @@
       </c>
     </row>
     <row r="100" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A100" s="9" t="s">
+      <c r="A100" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="B100" s="35" t="s">
+      <c r="B100" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C100" s="6"/>
@@ -11637,10 +11646,10 @@
       </c>
     </row>
     <row r="101" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A101" s="9" t="s">
+      <c r="A101" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="B101" s="35" t="s">
+      <c r="B101" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C101" s="6" t="s">
@@ -11693,10 +11702,10 @@
       </c>
     </row>
     <row r="102" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A102" s="9" t="s">
+      <c r="A102" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="B102" s="35" t="s">
+      <c r="B102" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C102" s="6" t="s">
@@ -11751,10 +11760,10 @@
       </c>
     </row>
     <row r="103" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A103" s="9" t="s">
+      <c r="A103" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="B103" s="35" t="s">
+      <c r="B103" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C103" s="6"/>
@@ -11791,10 +11800,10 @@
       </c>
     </row>
     <row r="104" spans="1:22" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A104" s="9" t="s">
+      <c r="A104" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="B104" s="35" t="s">
+      <c r="B104" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C104" s="6" t="s">
@@ -11843,10 +11852,10 @@
       </c>
     </row>
     <row r="105" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A105" s="9" t="s">
+      <c r="A105" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="B105" s="35" t="s">
+      <c r="B105" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C105" s="6" t="s">
@@ -11897,13 +11906,13 @@
       </c>
     </row>
     <row r="106" spans="1:22" ht="51" x14ac:dyDescent="0.25">
-      <c r="A106" s="9" t="s">
+      <c r="A106" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="B106" s="35" t="s">
+      <c r="B106" s="34" t="s">
         <v>607</v>
       </c>
-      <c r="C106" s="13"/>
+      <c r="C106" s="12"/>
       <c r="D106" s="6" t="s">
         <v>2</v>
       </c>
@@ -11913,14 +11922,14 @@
       <c r="F106" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G106" s="13"/>
-      <c r="H106" s="13">
+      <c r="G106" s="12"/>
+      <c r="H106" s="12">
         <v>2011</v>
       </c>
-      <c r="I106" s="13">
+      <c r="I106" s="12">
         <v>2009</v>
       </c>
-      <c r="J106" s="9">
+      <c r="J106" s="8">
         <v>2006</v>
       </c>
       <c r="K106" s="7" t="s">
@@ -11947,10 +11956,10 @@
       </c>
     </row>
     <row r="107" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A107" s="9" t="s">
+      <c r="A107" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="B107" s="35" t="s">
+      <c r="B107" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C107" s="6" t="s">
@@ -12001,10 +12010,10 @@
       </c>
     </row>
     <row r="108" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A108" s="9" t="s">
+      <c r="A108" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="B108" s="35" t="s">
+      <c r="B108" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C108" s="6" t="s">
@@ -12041,10 +12050,10 @@
       </c>
     </row>
     <row r="109" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A109" s="9" t="s">
+      <c r="A109" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="B109" s="35" t="s">
+      <c r="B109" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C109" s="6"/>
@@ -12083,10 +12092,10 @@
       </c>
     </row>
     <row r="110" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A110" s="9" t="s">
+      <c r="A110" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="B110" s="35" t="s">
+      <c r="B110" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C110" s="6"/>
@@ -12123,10 +12132,10 @@
       </c>
     </row>
     <row r="111" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A111" s="9" t="s">
+      <c r="A111" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="B111" s="35" t="s">
+      <c r="B111" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C111" s="4"/>
@@ -12161,10 +12170,10 @@
       </c>
     </row>
     <row r="112" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A112" s="9" t="s">
+      <c r="A112" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="B112" s="35" t="s">
+      <c r="B112" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C112" s="6"/>
@@ -12205,10 +12214,10 @@
       </c>
     </row>
     <row r="113" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A113" s="9" t="s">
+      <c r="A113" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="B113" s="35" t="s">
+      <c r="B113" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C113" s="6"/>
@@ -12243,10 +12252,10 @@
       </c>
     </row>
     <row r="114" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A114" s="9" t="s">
+      <c r="A114" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="B114" s="35" t="s">
+      <c r="B114" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C114" s="6" t="s">
@@ -12281,10 +12290,10 @@
       </c>
     </row>
     <row r="115" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A115" s="9" t="s">
+      <c r="A115" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="B115" s="35" t="s">
+      <c r="B115" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C115" s="6"/>
@@ -12323,10 +12332,10 @@
       </c>
     </row>
     <row r="116" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A116" s="9" t="s">
+      <c r="A116" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="B116" s="35" t="s">
+      <c r="B116" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C116" s="6" t="s">
@@ -12371,10 +12380,10 @@
       </c>
     </row>
     <row r="117" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A117" s="9" t="s">
+      <c r="A117" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="B117" s="35" t="s">
+      <c r="B117" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C117" s="6"/>
@@ -12411,10 +12420,10 @@
       </c>
     </row>
     <row r="118" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A118" s="9" t="s">
+      <c r="A118" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="B118" s="35" t="s">
+      <c r="B118" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C118" s="6" t="s">
@@ -12444,17 +12453,17 @@
       <c r="K118" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="L118" s="14"/>
-      <c r="M118" s="14"/>
+      <c r="L118" s="13"/>
+      <c r="M118" s="13"/>
       <c r="N118" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="O118" s="15"/>
-      <c r="P118" s="14"/>
-      <c r="Q118" s="14"/>
-      <c r="R118" s="14"/>
-      <c r="S118" s="14"/>
-      <c r="T118" s="15"/>
+      <c r="O118" s="14"/>
+      <c r="P118" s="13"/>
+      <c r="Q118" s="13"/>
+      <c r="R118" s="13"/>
+      <c r="S118" s="13"/>
+      <c r="T118" s="14"/>
       <c r="U118" s="7" t="s">
         <v>4</v>
       </c>
@@ -12463,10 +12472,10 @@
       </c>
     </row>
     <row r="119" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A119" s="9" t="s">
+      <c r="A119" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="B119" s="35" t="s">
+      <c r="B119" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C119" s="6"/>
@@ -12503,10 +12512,10 @@
       </c>
     </row>
     <row r="120" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A120" s="9" t="s">
+      <c r="A120" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="B120" s="35" t="s">
+      <c r="B120" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C120" s="6"/>
@@ -12541,10 +12550,10 @@
       </c>
     </row>
     <row r="121" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A121" s="9" t="s">
+      <c r="A121" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="B121" s="35" t="s">
+      <c r="B121" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C121" s="6" t="s">
@@ -12583,10 +12592,10 @@
       </c>
     </row>
     <row r="122" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A122" s="9" t="s">
+      <c r="A122" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="B122" s="35" t="s">
+      <c r="B122" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C122" s="6" t="s">
@@ -12621,10 +12630,10 @@
       </c>
     </row>
     <row r="123" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A123" s="9" t="s">
+      <c r="A123" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="B123" s="35" t="s">
+      <c r="B123" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C123" s="6"/>
@@ -12642,15 +12651,15 @@
       <c r="K123" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L123" s="14"/>
-      <c r="M123" s="14"/>
-      <c r="N123" s="14"/>
-      <c r="O123" s="15"/>
-      <c r="P123" s="14"/>
-      <c r="Q123" s="14"/>
-      <c r="R123" s="14"/>
-      <c r="S123" s="14"/>
-      <c r="T123" s="15"/>
+      <c r="L123" s="13"/>
+      <c r="M123" s="13"/>
+      <c r="N123" s="13"/>
+      <c r="O123" s="14"/>
+      <c r="P123" s="13"/>
+      <c r="Q123" s="13"/>
+      <c r="R123" s="13"/>
+      <c r="S123" s="13"/>
+      <c r="T123" s="14"/>
       <c r="U123" s="7" t="s">
         <v>144</v>
       </c>
@@ -12659,10 +12668,10 @@
       </c>
     </row>
     <row r="124" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A124" s="9" t="s">
+      <c r="A124" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="B124" s="35" t="s">
+      <c r="B124" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C124" s="6" t="s">
@@ -12699,10 +12708,10 @@
       </c>
     </row>
     <row r="125" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A125" s="9" t="s">
+      <c r="A125" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="B125" s="35" t="s">
+      <c r="B125" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C125" s="6" t="s">
@@ -12737,10 +12746,10 @@
       </c>
     </row>
     <row r="126" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A126" s="9" t="s">
+      <c r="A126" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="B126" s="35" t="s">
+      <c r="B126" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C126" s="6"/>
@@ -12777,10 +12786,10 @@
       </c>
     </row>
     <row r="127" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A127" s="9" t="s">
+      <c r="A127" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="B127" s="35" t="s">
+      <c r="B127" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C127" s="6"/>
@@ -12815,10 +12824,10 @@
       </c>
     </row>
     <row r="128" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A128" s="9" t="s">
+      <c r="A128" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="B128" s="35" t="s">
+      <c r="B128" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C128" s="6" t="s">
@@ -12863,10 +12872,10 @@
       </c>
     </row>
     <row r="129" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A129" s="9" t="s">
+      <c r="A129" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="B129" s="35" t="s">
+      <c r="B129" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C129" s="6" t="s">
@@ -12925,10 +12934,10 @@
       </c>
     </row>
     <row r="130" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A130" s="9" t="s">
+      <c r="A130" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="B130" s="35" t="s">
+      <c r="B130" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C130" s="6" t="s">
@@ -12973,10 +12982,10 @@
       </c>
     </row>
     <row r="131" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A131" s="9" t="s">
+      <c r="A131" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="B131" s="35" t="s">
+      <c r="B131" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C131" s="6" t="s">
@@ -13021,10 +13030,10 @@
       </c>
     </row>
     <row r="132" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A132" s="9" t="s">
+      <c r="A132" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="B132" s="35" t="s">
+      <c r="B132" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C132" s="6"/>
@@ -13061,10 +13070,10 @@
       </c>
     </row>
     <row r="133" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A133" s="9" t="s">
+      <c r="A133" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="B133" s="35" t="s">
+      <c r="B133" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C133" s="6" t="s">
@@ -13109,10 +13118,10 @@
       </c>
     </row>
     <row r="134" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A134" s="9" t="s">
+      <c r="A134" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="B134" s="35" t="s">
+      <c r="B134" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C134" s="6" t="s">
@@ -13167,10 +13176,10 @@
       </c>
     </row>
     <row r="135" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A135" s="9" t="s">
+      <c r="A135" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="B135" s="35" t="s">
+      <c r="B135" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C135" s="6" t="s">
@@ -13221,10 +13230,10 @@
       </c>
     </row>
     <row r="136" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A136" s="9" t="s">
+      <c r="A136" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="B136" s="35" t="s">
+      <c r="B136" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C136" s="6"/>
@@ -13269,10 +13278,10 @@
       </c>
     </row>
     <row r="137" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A137" s="9" t="s">
+      <c r="A137" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="B137" s="35" t="s">
+      <c r="B137" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C137" s="6"/>
@@ -13309,10 +13318,10 @@
       </c>
     </row>
     <row r="138" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A138" s="9" t="s">
+      <c r="A138" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="B138" s="35" t="s">
+      <c r="B138" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C138" s="4"/>
@@ -13347,10 +13356,10 @@
       </c>
     </row>
     <row r="139" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A139" s="9" t="s">
+      <c r="A139" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="B139" s="35" t="s">
+      <c r="B139" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C139" s="6"/>
@@ -13389,10 +13398,10 @@
       </c>
     </row>
     <row r="140" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A140" s="9" t="s">
+      <c r="A140" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="B140" s="35" t="s">
+      <c r="B140" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C140" s="6"/>
@@ -13431,10 +13440,10 @@
       </c>
     </row>
     <row r="141" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A141" s="9" t="s">
+      <c r="A141" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="B141" s="35" t="s">
+      <c r="B141" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C141" s="6"/>
@@ -13473,10 +13482,10 @@
       </c>
     </row>
     <row r="142" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A142" s="9" t="s">
+      <c r="A142" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="B142" s="35" t="s">
+      <c r="B142" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C142" s="6"/>
@@ -13515,10 +13524,10 @@
       </c>
     </row>
     <row r="143" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A143" s="9" t="s">
+      <c r="A143" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="B143" s="35" t="s">
+      <c r="B143" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C143" s="6" t="s">
@@ -13557,10 +13566,10 @@
       </c>
     </row>
     <row r="144" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A144" s="9" t="s">
+      <c r="A144" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B144" s="35" t="s">
+      <c r="B144" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C144" s="6"/>
@@ -13599,10 +13608,10 @@
       </c>
     </row>
     <row r="145" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A145" s="9" t="s">
+      <c r="A145" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="B145" s="35" t="s">
+      <c r="B145" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C145" s="6"/>
@@ -13639,10 +13648,10 @@
       </c>
     </row>
     <row r="146" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A146" s="9" t="s">
+      <c r="A146" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="B146" s="35" t="s">
+      <c r="B146" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C146" s="6" t="s">
@@ -13695,10 +13704,10 @@
       </c>
     </row>
     <row r="147" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A147" s="9" t="s">
+      <c r="A147" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="B147" s="35" t="s">
+      <c r="B147" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C147" s="6" t="s">
@@ -13743,10 +13752,10 @@
       </c>
     </row>
     <row r="148" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A148" s="9" t="s">
+      <c r="A148" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="B148" s="35" t="s">
+      <c r="B148" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C148" s="6" t="s">
@@ -13787,10 +13796,10 @@
       </c>
     </row>
     <row r="149" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A149" s="9" t="s">
+      <c r="A149" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="B149" s="35" t="s">
+      <c r="B149" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C149" s="6" t="s">
@@ -13833,10 +13842,10 @@
       </c>
     </row>
     <row r="150" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A150" s="9" t="s">
+      <c r="A150" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="B150" s="35" t="s">
+      <c r="B150" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C150" s="6" t="s">
@@ -13885,10 +13894,10 @@
       </c>
     </row>
     <row r="151" spans="1:22" ht="51" x14ac:dyDescent="0.25">
-      <c r="A151" s="9" t="s">
+      <c r="A151" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="B151" s="35" t="s">
+      <c r="B151" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C151" s="6"/>
@@ -13929,10 +13938,10 @@
       </c>
     </row>
     <row r="152" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A152" s="9" t="s">
+      <c r="A152" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="B152" s="35" t="s">
+      <c r="B152" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C152" s="6" t="s">
@@ -13969,10 +13978,10 @@
       </c>
     </row>
     <row r="153" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A153" s="9" t="s">
+      <c r="A153" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="B153" s="35" t="s">
+      <c r="B153" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C153" s="6"/>
@@ -14009,10 +14018,10 @@
       </c>
     </row>
     <row r="154" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A154" s="9" t="s">
+      <c r="A154" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="B154" s="35" t="s">
+      <c r="B154" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C154" s="6" t="s">
@@ -14069,10 +14078,10 @@
       </c>
     </row>
     <row r="155" spans="1:22" ht="51" x14ac:dyDescent="0.25">
-      <c r="A155" s="9" t="s">
+      <c r="A155" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="B155" s="35" t="s">
+      <c r="B155" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C155" s="6" t="s">
@@ -14081,34 +14090,34 @@
       <c r="D155" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E155" s="13"/>
+      <c r="E155" s="12"/>
       <c r="F155" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G155" s="13">
+      <c r="G155" s="12">
         <v>1980</v>
       </c>
-      <c r="H155" s="13" t="s">
+      <c r="H155" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="I155" s="13"/>
-      <c r="J155" s="9">
+      <c r="I155" s="12"/>
+      <c r="J155" s="8">
         <v>2008</v>
       </c>
-      <c r="K155" s="9" t="s">
+      <c r="K155" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="L155" s="16" t="s">
+      <c r="L155" s="15" t="s">
         <v>2</v>
       </c>
       <c r="M155" s="4"/>
       <c r="N155" s="4"/>
-      <c r="O155" s="17" t="s">
+      <c r="O155" s="16" t="s">
         <v>2</v>
       </c>
       <c r="P155" s="4"/>
       <c r="Q155" s="4"/>
-      <c r="R155" s="16" t="s">
+      <c r="R155" s="15" t="s">
         <v>2</v>
       </c>
       <c r="S155" s="4"/>
@@ -14121,10 +14130,10 @@
       </c>
     </row>
     <row r="156" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A156" s="9" t="s">
+      <c r="A156" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="B156" s="35" t="s">
+      <c r="B156" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C156" s="6" t="s">
@@ -14161,29 +14170,29 @@
       </c>
     </row>
     <row r="157" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A157" s="9" t="s">
+      <c r="A157" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="B157" s="35" t="s">
+      <c r="B157" s="34" t="s">
         <v>607</v>
       </c>
-      <c r="C157" s="13"/>
+      <c r="C157" s="12"/>
       <c r="D157" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E157" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F157" s="9"/>
-      <c r="G157" s="13"/>
-      <c r="H157" s="13">
+      <c r="F157" s="8"/>
+      <c r="G157" s="12"/>
+      <c r="H157" s="12">
         <v>1985</v>
       </c>
-      <c r="I157" s="13">
+      <c r="I157" s="12">
         <v>1999</v>
       </c>
-      <c r="J157" s="9"/>
-      <c r="K157" s="9" t="s">
+      <c r="J157" s="8"/>
+      <c r="K157" s="8" t="s">
         <v>19</v>
       </c>
       <c r="L157" s="4"/>
@@ -14205,10 +14214,10 @@
       </c>
     </row>
     <row r="158" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A158" s="9" t="s">
+      <c r="A158" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="B158" s="35" t="s">
+      <c r="B158" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C158" s="6"/>
@@ -14243,10 +14252,10 @@
       </c>
     </row>
     <row r="159" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A159" s="9" t="s">
+      <c r="A159" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="B159" s="35" t="s">
+      <c r="B159" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C159" s="6" t="s">
@@ -14283,10 +14292,10 @@
       </c>
     </row>
     <row r="160" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A160" s="9" t="s">
+      <c r="A160" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="B160" s="35" t="s">
+      <c r="B160" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C160" s="6" t="s">
@@ -14329,10 +14338,10 @@
       </c>
     </row>
     <row r="161" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A161" s="9" t="s">
+      <c r="A161" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="B161" s="35" t="s">
+      <c r="B161" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C161" s="6" t="s">
@@ -14375,10 +14384,10 @@
       </c>
     </row>
     <row r="162" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A162" s="9" t="s">
+      <c r="A162" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="B162" s="35" t="s">
+      <c r="B162" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C162" s="6" t="s">
@@ -14421,10 +14430,10 @@
       </c>
     </row>
     <row r="163" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A163" s="9" t="s">
+      <c r="A163" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="B163" s="35" t="s">
+      <c r="B163" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C163" s="6" t="s">
@@ -14456,10 +14465,10 @@
       </c>
       <c r="L163" s="4"/>
       <c r="M163" s="4"/>
-      <c r="N163" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="O163" s="17" t="s">
+      <c r="N163" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="O163" s="16" t="s">
         <v>2</v>
       </c>
       <c r="P163" s="4"/>
@@ -14475,10 +14484,10 @@
       </c>
     </row>
     <row r="164" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A164" s="9" t="s">
+      <c r="A164" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="B164" s="35" t="s">
+      <c r="B164" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C164" s="6" t="s">
@@ -14513,10 +14522,10 @@
       </c>
     </row>
     <row r="165" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A165" s="9" t="s">
+      <c r="A165" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="B165" s="35" t="s">
+      <c r="B165" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C165" s="6" t="s">
@@ -14559,10 +14568,10 @@
       </c>
     </row>
     <row r="166" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A166" s="9" t="s">
+      <c r="A166" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="B166" s="35" t="s">
+      <c r="B166" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C166" s="6" t="s">
@@ -14584,17 +14593,17 @@
       <c r="K166" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="L166" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="M166" s="16" t="s">
+      <c r="L166" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="M166" s="15" t="s">
         <v>2</v>
       </c>
       <c r="N166" s="4"/>
       <c r="O166" s="5"/>
       <c r="P166" s="4"/>
       <c r="Q166" s="4"/>
-      <c r="R166" s="16" t="s">
+      <c r="R166" s="15" t="s">
         <v>2</v>
       </c>
       <c r="S166" s="4"/>
@@ -14607,10 +14616,10 @@
       </c>
     </row>
     <row r="167" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A167" s="9" t="s">
+      <c r="A167" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="B167" s="35" t="s">
+      <c r="B167" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C167" s="6" t="s">
@@ -14629,14 +14638,14 @@
         <v>3</v>
       </c>
       <c r="L167" s="4"/>
-      <c r="M167" s="16" t="s">
+      <c r="M167" s="15" t="s">
         <v>2</v>
       </c>
       <c r="N167" s="4"/>
       <c r="O167" s="5"/>
       <c r="P167" s="4"/>
       <c r="Q167" s="4"/>
-      <c r="R167" s="16" t="s">
+      <c r="R167" s="15" t="s">
         <v>2</v>
       </c>
       <c r="S167" s="4"/>
@@ -14649,10 +14658,10 @@
       </c>
     </row>
     <row r="168" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A168" s="9" t="s">
+      <c r="A168" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="B168" s="35" t="s">
+      <c r="B168" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C168" s="6" t="s">
@@ -14678,7 +14687,7 @@
       </c>
       <c r="L168" s="4"/>
       <c r="M168" s="4"/>
-      <c r="N168" s="16" t="s">
+      <c r="N168" s="15" t="s">
         <v>2</v>
       </c>
       <c r="O168" s="5"/>
@@ -14695,10 +14704,10 @@
       </c>
     </row>
     <row r="169" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A169" s="9" t="s">
+      <c r="A169" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="B169" s="35" t="s">
+      <c r="B169" s="34" t="s">
         <v>607</v>
       </c>
       <c r="C169" s="6" t="s">
@@ -14726,13 +14735,13 @@
       </c>
       <c r="L169" s="4"/>
       <c r="M169" s="4"/>
-      <c r="N169" s="16" t="s">
+      <c r="N169" s="15" t="s">
         <v>2</v>
       </c>
       <c r="O169" s="5"/>
       <c r="P169" s="4"/>
       <c r="Q169" s="4"/>
-      <c r="R169" s="16"/>
+      <c r="R169" s="15"/>
       <c r="S169" s="4"/>
       <c r="T169" s="5"/>
       <c r="U169" s="7" t="s">
@@ -14743,54 +14752,54 @@
       </c>
     </row>
     <row r="170" spans="1:22" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="18" t="s">
+      <c r="A170" s="17" t="s">
         <v>296</v>
       </c>
-      <c r="B170" s="35" t="s">
+      <c r="B170" s="34" t="s">
         <v>607</v>
       </c>
-      <c r="C170" s="11"/>
-      <c r="D170" s="11"/>
-      <c r="E170" s="11"/>
-      <c r="F170" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="G170" s="11"/>
-      <c r="H170" s="11"/>
-      <c r="I170" s="11"/>
-      <c r="J170" s="12">
+      <c r="C170" s="10"/>
+      <c r="D170" s="10"/>
+      <c r="E170" s="10"/>
+      <c r="F170" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G170" s="10"/>
+      <c r="H170" s="10"/>
+      <c r="I170" s="10"/>
+      <c r="J170" s="11">
         <v>2006</v>
       </c>
-      <c r="K170" s="12" t="s">
+      <c r="K170" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="L170" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="M170" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="N170" s="20"/>
-      <c r="O170" s="21"/>
-      <c r="P170" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q170" s="20"/>
-      <c r="R170" s="20"/>
-      <c r="S170" s="20"/>
-      <c r="T170" s="21"/>
-      <c r="U170" s="12" t="s">
+      <c r="L170" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="M170" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="N170" s="19"/>
+      <c r="O170" s="20"/>
+      <c r="P170" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q170" s="19"/>
+      <c r="R170" s="19"/>
+      <c r="S170" s="19"/>
+      <c r="T170" s="20"/>
+      <c r="U170" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="V170" s="11">
+      <c r="V170" s="10">
         <v>27</v>
       </c>
     </row>
     <row r="171" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A171" s="9" t="s">
+      <c r="A171" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="B171" s="35" t="s">
+      <c r="B171" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C171" s="4"/>
@@ -14825,10 +14834,10 @@
       </c>
     </row>
     <row r="172" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A172" s="9" t="s">
+      <c r="A172" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="B172" s="35" t="s">
+      <c r="B172" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C172" s="4" t="s">
@@ -14854,21 +14863,21 @@
       <c r="K172" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L172" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="M172" s="16" t="s">
+      <c r="L172" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="M172" s="15" t="s">
         <v>2</v>
       </c>
       <c r="N172" s="4"/>
-      <c r="O172" s="17" t="s">
+      <c r="O172" s="16" t="s">
         <v>2</v>
       </c>
       <c r="P172" s="4"/>
-      <c r="Q172" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="R172" s="16" t="s">
+      <c r="Q172" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="R172" s="15" t="s">
         <v>2</v>
       </c>
       <c r="S172" s="4"/>
@@ -14881,10 +14890,10 @@
       </c>
     </row>
     <row r="173" spans="1:22" ht="51" x14ac:dyDescent="0.25">
-      <c r="A173" s="9" t="s">
+      <c r="A173" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="B173" s="35" t="s">
+      <c r="B173" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C173" s="4"/>
@@ -14925,10 +14934,10 @@
       </c>
     </row>
     <row r="174" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A174" s="9" t="s">
+      <c r="A174" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="B174" s="35" t="s">
+      <c r="B174" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C174" s="4" t="s">
@@ -14981,10 +14990,10 @@
       </c>
     </row>
     <row r="175" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A175" s="9" t="s">
+      <c r="A175" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="B175" s="35" t="s">
+      <c r="B175" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C175" s="4"/>
@@ -15019,10 +15028,10 @@
       </c>
     </row>
     <row r="176" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A176" s="9" t="s">
+      <c r="A176" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="B176" s="35" t="s">
+      <c r="B176" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C176" s="4" t="s">
@@ -15067,10 +15076,10 @@
       </c>
     </row>
     <row r="177" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A177" s="9" t="s">
+      <c r="A177" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="B177" s="35" t="s">
+      <c r="B177" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C177" s="4" t="s">
@@ -15109,10 +15118,10 @@
       </c>
     </row>
     <row r="178" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A178" s="9" t="s">
+      <c r="A178" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="B178" s="35" t="s">
+      <c r="B178" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C178" s="4" t="s">
@@ -15169,10 +15178,10 @@
       </c>
     </row>
     <row r="179" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A179" s="9" t="s">
+      <c r="A179" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="B179" s="35" t="s">
+      <c r="B179" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C179" s="4" t="s">
@@ -15221,10 +15230,10 @@
       </c>
     </row>
     <row r="180" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A180" s="9" t="s">
+      <c r="A180" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="B180" s="35" t="s">
+      <c r="B180" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C180" s="4"/>
@@ -15263,10 +15272,10 @@
       </c>
     </row>
     <row r="181" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A181" s="9" t="s">
+      <c r="A181" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="B181" s="35" t="s">
+      <c r="B181" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C181" s="4"/>
@@ -15307,10 +15316,10 @@
       </c>
     </row>
     <row r="182" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A182" s="9" t="s">
+      <c r="A182" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="B182" s="35" t="s">
+      <c r="B182" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C182" s="4" t="s">
@@ -15351,10 +15360,10 @@
       </c>
     </row>
     <row r="183" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A183" s="9" t="s">
+      <c r="A183" s="8" t="s">
         <v>322</v>
       </c>
-      <c r="B183" s="35" t="s">
+      <c r="B183" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C183" s="4" t="s">
@@ -15389,10 +15398,10 @@
       </c>
     </row>
     <row r="184" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A184" s="9" t="s">
+      <c r="A184" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="B184" s="35" t="s">
+      <c r="B184" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C184" s="4" t="s">
@@ -15449,10 +15458,10 @@
       </c>
     </row>
     <row r="185" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A185" s="9" t="s">
+      <c r="A185" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="B185" s="35" t="s">
+      <c r="B185" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C185" s="4" t="s">
@@ -15505,10 +15514,10 @@
       </c>
     </row>
     <row r="186" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A186" s="9" t="s">
+      <c r="A186" s="8" t="s">
         <v>327</v>
       </c>
-      <c r="B186" s="35" t="s">
+      <c r="B186" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C186" s="4" t="s">
@@ -15549,10 +15558,10 @@
       </c>
     </row>
     <row r="187" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A187" s="9" t="s">
+      <c r="A187" s="8" t="s">
         <v>329</v>
       </c>
-      <c r="B187" s="35" t="s">
+      <c r="B187" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C187" s="4"/>
@@ -15587,10 +15596,10 @@
       </c>
     </row>
     <row r="188" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A188" s="9" t="s">
+      <c r="A188" s="8" t="s">
         <v>330</v>
       </c>
-      <c r="B188" s="35" t="s">
+      <c r="B188" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C188" s="4" t="s">
@@ -15631,10 +15640,10 @@
       </c>
     </row>
     <row r="189" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A189" s="9" t="s">
+      <c r="A189" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="B189" s="35" t="s">
+      <c r="B189" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C189" s="4"/>
@@ -15685,10 +15694,10 @@
       </c>
     </row>
     <row r="190" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A190" s="9" t="s">
+      <c r="A190" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="B190" s="35" t="s">
+      <c r="B190" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C190" s="4" t="s">
@@ -15735,10 +15744,10 @@
       </c>
     </row>
     <row r="191" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A191" s="9" t="s">
+      <c r="A191" s="8" t="s">
         <v>335</v>
       </c>
-      <c r="B191" s="35" t="s">
+      <c r="B191" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C191" s="4" t="s">
@@ -15785,10 +15794,10 @@
       </c>
     </row>
     <row r="192" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A192" s="9" t="s">
+      <c r="A192" s="8" t="s">
         <v>337</v>
       </c>
-      <c r="B192" s="35" t="s">
+      <c r="B192" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C192" s="4"/>
@@ -15835,10 +15844,10 @@
       </c>
     </row>
     <row r="193" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A193" s="9" t="s">
+      <c r="A193" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="B193" s="35" t="s">
+      <c r="B193" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C193" s="4"/>
@@ -15873,10 +15882,10 @@
       </c>
     </row>
     <row r="194" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A194" s="9" t="s">
+      <c r="A194" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="B194" s="35" t="s">
+      <c r="B194" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C194" s="4"/>
@@ -15915,10 +15924,10 @@
       </c>
     </row>
     <row r="195" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A195" s="9" t="s">
+      <c r="A195" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="B195" s="35" t="s">
+      <c r="B195" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C195" s="4"/>
@@ -15963,10 +15972,10 @@
       </c>
     </row>
     <row r="196" spans="1:22" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A196" s="9" t="s">
+      <c r="A196" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="B196" s="35" t="s">
+      <c r="B196" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C196" s="4" t="s">
@@ -16023,10 +16032,10 @@
       </c>
     </row>
     <row r="197" spans="1:22" ht="51" x14ac:dyDescent="0.25">
-      <c r="A197" s="9" t="s">
+      <c r="A197" s="8" t="s">
         <v>347</v>
       </c>
-      <c r="B197" s="35" t="s">
+      <c r="B197" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C197" s="4" t="s">
@@ -16061,10 +16070,10 @@
       </c>
     </row>
     <row r="198" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A198" s="9" t="s">
+      <c r="A198" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="B198" s="35" t="s">
+      <c r="B198" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C198" s="4"/>
@@ -16103,10 +16112,10 @@
       </c>
     </row>
     <row r="199" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A199" s="9" t="s">
+      <c r="A199" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="B199" s="35" t="s">
+      <c r="B199" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C199" s="4"/>
@@ -16147,10 +16156,10 @@
       </c>
     </row>
     <row r="200" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A200" s="9" t="s">
+      <c r="A200" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="B200" s="35" t="s">
+      <c r="B200" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C200" s="4" t="s">
@@ -16197,62 +16206,62 @@
       </c>
     </row>
     <row r="201" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="33" t="s">
+      <c r="A201" s="32" t="s">
         <v>354</v>
       </c>
-      <c r="B201" s="35" t="s">
+      <c r="B201" s="34" t="s">
         <v>608</v>
       </c>
-      <c r="C201" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="D201" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="E201" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="F201" s="30"/>
-      <c r="G201" s="28">
+      <c r="C201" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D201" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E201" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F201" s="29"/>
+      <c r="G201" s="27">
         <v>1900</v>
       </c>
-      <c r="H201" s="29" t="s">
+      <c r="H201" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="I201" s="29">
+      <c r="I201" s="28">
         <v>1954</v>
       </c>
-      <c r="J201" s="30"/>
-      <c r="K201" s="32" t="s">
+      <c r="J201" s="29"/>
+      <c r="K201" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="L201" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="M201" s="29"/>
-      <c r="N201" s="29"/>
-      <c r="O201" s="30"/>
-      <c r="P201" s="28"/>
-      <c r="Q201" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="R201" s="29"/>
-      <c r="S201" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="T201" s="30"/>
-      <c r="U201" s="31" t="s">
+      <c r="L201" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="M201" s="28"/>
+      <c r="N201" s="28"/>
+      <c r="O201" s="29"/>
+      <c r="P201" s="27"/>
+      <c r="Q201" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="R201" s="28"/>
+      <c r="S201" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="T201" s="29"/>
+      <c r="U201" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="V201" s="27" t="s">
+      <c r="V201" s="26" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="202" spans="1:22" ht="51" x14ac:dyDescent="0.25">
-      <c r="A202" s="9" t="s">
+      <c r="A202" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="B202" s="35" t="s">
+      <c r="B202" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C202" s="4" t="s">
@@ -16311,10 +16320,10 @@
       </c>
     </row>
     <row r="203" spans="1:22" ht="51" x14ac:dyDescent="0.25">
-      <c r="A203" s="9" t="s">
+      <c r="A203" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="B203" s="35" t="s">
+      <c r="B203" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C203" s="4" t="s">
@@ -16371,10 +16380,10 @@
       </c>
     </row>
     <row r="204" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A204" s="9" t="s">
+      <c r="A204" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="B204" s="35" t="s">
+      <c r="B204" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C204" s="4" t="s">
@@ -16413,10 +16422,10 @@
       </c>
     </row>
     <row r="205" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A205" s="9" t="s">
+      <c r="A205" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="B205" s="35" t="s">
+      <c r="B205" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C205" s="4" t="s">
@@ -16469,10 +16478,10 @@
       </c>
     </row>
     <row r="206" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A206" s="9" t="s">
+      <c r="A206" s="8" t="s">
         <v>361</v>
       </c>
-      <c r="B206" s="35" t="s">
+      <c r="B206" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C206" s="4" t="s">
@@ -16529,10 +16538,10 @@
       </c>
     </row>
     <row r="207" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A207" s="9" t="s">
+      <c r="A207" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="B207" s="35" t="s">
+      <c r="B207" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C207" s="4" t="s">
@@ -16585,10 +16594,10 @@
       </c>
     </row>
     <row r="208" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A208" s="9" t="s">
+      <c r="A208" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="B208" s="35" t="s">
+      <c r="B208" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C208" s="4" t="s">
@@ -16643,10 +16652,10 @@
       </c>
     </row>
     <row r="209" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A209" s="9" t="s">
+      <c r="A209" s="8" t="s">
         <v>366</v>
       </c>
-      <c r="B209" s="35" t="s">
+      <c r="B209" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C209" s="4" t="s">
@@ -16685,10 +16694,10 @@
       </c>
     </row>
     <row r="210" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A210" s="9" t="s">
+      <c r="A210" s="8" t="s">
         <v>368</v>
       </c>
-      <c r="B210" s="35" t="s">
+      <c r="B210" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C210" s="4"/>
@@ -16733,10 +16742,10 @@
       </c>
     </row>
     <row r="211" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A211" s="9" t="s">
+      <c r="A211" s="8" t="s">
         <v>370</v>
       </c>
-      <c r="B211" s="35" t="s">
+      <c r="B211" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C211" s="4" t="s">
@@ -16787,10 +16796,10 @@
       </c>
     </row>
     <row r="212" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A212" s="9" t="s">
+      <c r="A212" s="8" t="s">
         <v>371</v>
       </c>
-      <c r="B212" s="35" t="s">
+      <c r="B212" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C212" s="4" t="s">
@@ -16847,10 +16856,10 @@
       </c>
     </row>
     <row r="213" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A213" s="9" t="s">
+      <c r="A213" s="8" t="s">
         <v>373</v>
       </c>
-      <c r="B213" s="35" t="s">
+      <c r="B213" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C213" s="4"/>
@@ -16891,10 +16900,10 @@
       </c>
     </row>
     <row r="214" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A214" s="9" t="s">
+      <c r="A214" s="8" t="s">
         <v>375</v>
       </c>
-      <c r="B214" s="35" t="s">
+      <c r="B214" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C214" s="4" t="s">
@@ -16935,10 +16944,10 @@
       </c>
     </row>
     <row r="215" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A215" s="9" t="s">
+      <c r="A215" s="8" t="s">
         <v>377</v>
       </c>
-      <c r="B215" s="35" t="s">
+      <c r="B215" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C215" s="4" t="s">
@@ -16981,10 +16990,10 @@
       </c>
     </row>
     <row r="216" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A216" s="9" t="s">
+      <c r="A216" s="8" t="s">
         <v>379</v>
       </c>
-      <c r="B216" s="35" t="s">
+      <c r="B216" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C216" s="4"/>
@@ -17019,10 +17028,10 @@
       </c>
     </row>
     <row r="217" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A217" s="9" t="s">
+      <c r="A217" s="8" t="s">
         <v>380</v>
       </c>
-      <c r="B217" s="35" t="s">
+      <c r="B217" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C217" s="4"/>
@@ -17057,10 +17066,10 @@
       </c>
     </row>
     <row r="218" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A218" s="9" t="s">
+      <c r="A218" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="B218" s="35" t="s">
+      <c r="B218" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C218" s="4"/>
@@ -17107,10 +17116,10 @@
       </c>
     </row>
     <row r="219" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A219" s="9" t="s">
+      <c r="A219" s="8" t="s">
         <v>383</v>
       </c>
-      <c r="B219" s="35" t="s">
+      <c r="B219" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C219" s="4" t="s">
@@ -17149,10 +17158,10 @@
       </c>
     </row>
     <row r="220" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A220" s="9" t="s">
+      <c r="A220" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="B220" s="35" t="s">
+      <c r="B220" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C220" s="4" t="s">
@@ -17197,10 +17206,10 @@
       </c>
     </row>
     <row r="221" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A221" s="9" t="s">
+      <c r="A221" s="8" t="s">
         <v>387</v>
       </c>
-      <c r="B221" s="35" t="s">
+      <c r="B221" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C221" s="4" t="s">
@@ -17241,10 +17250,10 @@
       </c>
     </row>
     <row r="222" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A222" s="9" t="s">
+      <c r="A222" s="8" t="s">
         <v>389</v>
       </c>
-      <c r="B222" s="35" t="s">
+      <c r="B222" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C222" s="4" t="s">
@@ -17299,10 +17308,10 @@
       </c>
     </row>
     <row r="223" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A223" s="9" t="s">
+      <c r="A223" s="8" t="s">
         <v>391</v>
       </c>
-      <c r="B223" s="35" t="s">
+      <c r="B223" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C223" s="4" t="s">
@@ -17355,10 +17364,10 @@
       </c>
     </row>
     <row r="224" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A224" s="9" t="s">
+      <c r="A224" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="B224" s="35" t="s">
+      <c r="B224" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C224" s="4" t="s">
@@ -17411,10 +17420,10 @@
       </c>
     </row>
     <row r="225" spans="1:22" ht="51" x14ac:dyDescent="0.25">
-      <c r="A225" s="9" t="s">
+      <c r="A225" s="8" t="s">
         <v>396</v>
       </c>
-      <c r="B225" s="35" t="s">
+      <c r="B225" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C225" s="4" t="s">
@@ -17453,10 +17462,10 @@
       </c>
     </row>
     <row r="226" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A226" s="9" t="s">
+      <c r="A226" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="B226" s="35" t="s">
+      <c r="B226" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C226" s="4" t="s">
@@ -17495,10 +17504,10 @@
       </c>
     </row>
     <row r="227" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A227" s="9" t="s">
+      <c r="A227" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="B227" s="35" t="s">
+      <c r="B227" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C227" s="4" t="s">
@@ -17539,10 +17548,10 @@
       </c>
     </row>
     <row r="228" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A228" s="9" t="s">
+      <c r="A228" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="B228" s="35" t="s">
+      <c r="B228" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C228" s="4"/>
@@ -17579,10 +17588,10 @@
       </c>
     </row>
     <row r="229" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A229" s="9" t="s">
+      <c r="A229" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="B229" s="35" t="s">
+      <c r="B229" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C229" s="4"/>
@@ -17621,10 +17630,10 @@
       </c>
     </row>
     <row r="230" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A230" s="9" t="s">
+      <c r="A230" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="B230" s="35" t="s">
+      <c r="B230" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C230" s="4" t="s">
@@ -17685,10 +17694,10 @@
       </c>
     </row>
     <row r="231" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A231" s="9" t="s">
+      <c r="A231" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="B231" s="35" t="s">
+      <c r="B231" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C231" s="4"/>
@@ -17723,10 +17732,10 @@
       </c>
     </row>
     <row r="232" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A232" s="9" t="s">
+      <c r="A232" s="8" t="s">
         <v>404</v>
       </c>
-      <c r="B232" s="35" t="s">
+      <c r="B232" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C232" s="4" t="s">
@@ -17777,10 +17786,10 @@
       </c>
     </row>
     <row r="233" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A233" s="9" t="s">
+      <c r="A233" s="8" t="s">
         <v>406</v>
       </c>
-      <c r="B233" s="35" t="s">
+      <c r="B233" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C233" s="4"/>
@@ -17806,19 +17815,19 @@
       <c r="K233" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="L233" s="14"/>
-      <c r="M233" s="14"/>
+      <c r="L233" s="13"/>
+      <c r="M233" s="13"/>
       <c r="N233" s="4" t="s">
         <v>2</v>
       </c>
       <c r="O233" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="P233" s="14"/>
-      <c r="Q233" s="14"/>
-      <c r="R233" s="14"/>
-      <c r="S233" s="14"/>
-      <c r="T233" s="15"/>
+      <c r="P233" s="13"/>
+      <c r="Q233" s="13"/>
+      <c r="R233" s="13"/>
+      <c r="S233" s="13"/>
+      <c r="T233" s="14"/>
       <c r="U233" s="7" t="s">
         <v>40</v>
       </c>
@@ -17827,10 +17836,10 @@
       </c>
     </row>
     <row r="234" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A234" s="9" t="s">
+      <c r="A234" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="B234" s="35" t="s">
+      <c r="B234" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C234" s="4" t="s">
@@ -17889,10 +17898,10 @@
       </c>
     </row>
     <row r="235" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A235" s="9" t="s">
+      <c r="A235" s="8" t="s">
         <v>410</v>
       </c>
-      <c r="B235" s="35" t="s">
+      <c r="B235" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C235" s="4" t="s">
@@ -17935,10 +17944,10 @@
       </c>
     </row>
     <row r="236" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A236" s="9" t="s">
+      <c r="A236" s="8" t="s">
         <v>412</v>
       </c>
-      <c r="B236" s="35" t="s">
+      <c r="B236" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C236" s="4" t="s">
@@ -17973,10 +17982,10 @@
       </c>
     </row>
     <row r="237" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A237" s="9" t="s">
+      <c r="A237" s="8" t="s">
         <v>413</v>
       </c>
-      <c r="B237" s="35" t="s">
+      <c r="B237" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C237" s="4"/>
@@ -18011,10 +18020,10 @@
       </c>
     </row>
     <row r="238" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A238" s="9" t="s">
+      <c r="A238" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="B238" s="35" t="s">
+      <c r="B238" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C238" s="4" t="s">
@@ -18053,10 +18062,10 @@
       </c>
     </row>
     <row r="239" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A239" s="9" t="s">
+      <c r="A239" s="8" t="s">
         <v>415</v>
       </c>
-      <c r="B239" s="35" t="s">
+      <c r="B239" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C239" s="4"/>
@@ -18103,38 +18112,38 @@
       </c>
     </row>
     <row r="240" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A240" s="9" t="s">
+      <c r="A240" s="8" t="s">
         <v>418</v>
       </c>
-      <c r="B240" s="35" t="s">
+      <c r="B240" s="34" t="s">
         <v>608</v>
       </c>
-      <c r="C240" s="28"/>
-      <c r="D240" s="29"/>
-      <c r="E240" s="29"/>
-      <c r="F240" s="30"/>
-      <c r="G240" s="28"/>
-      <c r="H240" s="29"/>
-      <c r="I240" s="29"/>
-      <c r="J240" s="30"/>
-      <c r="K240" s="32"/>
-      <c r="L240" s="28"/>
-      <c r="M240" s="29"/>
-      <c r="N240" s="29"/>
-      <c r="O240" s="30"/>
-      <c r="P240" s="28"/>
-      <c r="Q240" s="29"/>
-      <c r="R240" s="29"/>
-      <c r="S240" s="29"/>
-      <c r="T240" s="30"/>
-      <c r="U240" s="31"/>
-      <c r="V240" s="27"/>
+      <c r="C240" s="27"/>
+      <c r="D240" s="28"/>
+      <c r="E240" s="28"/>
+      <c r="F240" s="29"/>
+      <c r="G240" s="27"/>
+      <c r="H240" s="28"/>
+      <c r="I240" s="28"/>
+      <c r="J240" s="29"/>
+      <c r="K240" s="31"/>
+      <c r="L240" s="27"/>
+      <c r="M240" s="28"/>
+      <c r="N240" s="28"/>
+      <c r="O240" s="29"/>
+      <c r="P240" s="27"/>
+      <c r="Q240" s="28"/>
+      <c r="R240" s="28"/>
+      <c r="S240" s="28"/>
+      <c r="T240" s="29"/>
+      <c r="U240" s="30"/>
+      <c r="V240" s="26"/>
     </row>
     <row r="241" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A241" s="9" t="s">
+      <c r="A241" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="B241" s="35" t="s">
+      <c r="B241" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C241" s="4" t="s">
@@ -18173,10 +18182,10 @@
       </c>
     </row>
     <row r="242" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A242" s="9" t="s">
+      <c r="A242" s="8" t="s">
         <v>420</v>
       </c>
-      <c r="B242" s="35" t="s">
+      <c r="B242" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C242" s="4" t="s">
@@ -18219,10 +18228,10 @@
       </c>
     </row>
     <row r="243" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A243" s="9" t="s">
+      <c r="A243" s="8" t="s">
         <v>421</v>
       </c>
-      <c r="B243" s="35" t="s">
+      <c r="B243" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C243" s="4" t="s">
@@ -18277,10 +18286,10 @@
       </c>
     </row>
     <row r="244" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A244" s="9" t="s">
+      <c r="A244" s="8" t="s">
         <v>423</v>
       </c>
-      <c r="B244" s="35" t="s">
+      <c r="B244" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C244" s="4" t="s">
@@ -18315,10 +18324,10 @@
       </c>
     </row>
     <row r="245" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A245" s="9" t="s">
+      <c r="A245" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="B245" s="35" t="s">
+      <c r="B245" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C245" s="4"/>
@@ -18357,10 +18366,10 @@
       </c>
     </row>
     <row r="246" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A246" s="9" t="s">
+      <c r="A246" s="8" t="s">
         <v>425</v>
       </c>
-      <c r="B246" s="35" t="s">
+      <c r="B246" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C246" s="4" t="s">
@@ -18413,10 +18422,10 @@
       </c>
     </row>
     <row r="247" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A247" s="9" t="s">
+      <c r="A247" s="8" t="s">
         <v>426</v>
       </c>
-      <c r="B247" s="35" t="s">
+      <c r="B247" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C247" s="4"/>
@@ -18455,10 +18464,10 @@
       </c>
     </row>
     <row r="248" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A248" s="9" t="s">
+      <c r="A248" s="8" t="s">
         <v>429</v>
       </c>
-      <c r="B248" s="35" t="s">
+      <c r="B248" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C248" s="4"/>
@@ -18497,10 +18506,10 @@
       </c>
     </row>
     <row r="249" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A249" s="9" t="s">
+      <c r="A249" s="8" t="s">
         <v>430</v>
       </c>
-      <c r="B249" s="35" t="s">
+      <c r="B249" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C249" s="4" t="s">
@@ -18539,10 +18548,10 @@
       </c>
     </row>
     <row r="250" spans="1:22" ht="51" x14ac:dyDescent="0.25">
-      <c r="A250" s="9" t="s">
+      <c r="A250" s="8" t="s">
         <v>432</v>
       </c>
-      <c r="B250" s="35" t="s">
+      <c r="B250" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C250" s="4"/>
@@ -18583,10 +18592,10 @@
       </c>
     </row>
     <row r="251" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A251" s="9" t="s">
+      <c r="A251" s="8" t="s">
         <v>433</v>
       </c>
-      <c r="B251" s="35" t="s">
+      <c r="B251" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C251" s="4" t="s">
@@ -18629,10 +18638,10 @@
       </c>
     </row>
     <row r="252" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A252" s="9" t="s">
+      <c r="A252" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="B252" s="35" t="s">
+      <c r="B252" s="34" t="s">
         <v>608</v>
       </c>
       <c r="C252" s="4"/>
@@ -18683,48 +18692,48 @@
       </c>
     </row>
     <row r="253" spans="1:22" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A253" s="18" t="s">
+      <c r="A253" s="17" t="s">
         <v>436</v>
       </c>
-      <c r="B253" s="35" t="s">
+      <c r="B253" s="34" t="s">
         <v>608</v>
       </c>
-      <c r="C253" s="20"/>
-      <c r="D253" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="E253" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F253" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="G253" s="20"/>
-      <c r="H253" s="22">
+      <c r="C253" s="19"/>
+      <c r="D253" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E253" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F253" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="G253" s="19"/>
+      <c r="H253" s="21">
         <v>1990</v>
       </c>
-      <c r="I253" s="22">
+      <c r="I253" s="21">
         <v>2001</v>
       </c>
-      <c r="J253" s="23" t="s">
+      <c r="J253" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="K253" s="23" t="s">
+      <c r="K253" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="L253" s="20"/>
-      <c r="M253" s="20"/>
-      <c r="N253" s="20"/>
-      <c r="O253" s="21"/>
-      <c r="P253" s="20"/>
-      <c r="Q253" s="20"/>
-      <c r="R253" s="20"/>
-      <c r="S253" s="20"/>
-      <c r="T253" s="21"/>
-      <c r="U253" s="12" t="s">
+      <c r="L253" s="19"/>
+      <c r="M253" s="19"/>
+      <c r="N253" s="19"/>
+      <c r="O253" s="20"/>
+      <c r="P253" s="19"/>
+      <c r="Q253" s="19"/>
+      <c r="R253" s="19"/>
+      <c r="S253" s="19"/>
+      <c r="T253" s="20"/>
+      <c r="U253" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="V253" s="11" t="s">
+      <c r="V253" s="10" t="s">
         <v>395</v>
       </c>
     </row>
@@ -18732,7 +18741,7 @@
       <c r="A254" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="B254" s="34" t="s">
+      <c r="B254" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C254" s="6" t="s">
@@ -18792,7 +18801,7 @@
       <c r="A255" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="B255" s="34" t="s">
+      <c r="B255" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C255" s="6" t="s">
@@ -18850,7 +18859,7 @@
       <c r="A256" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="B256" s="34" t="s">
+      <c r="B256" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C256" s="6" t="s">
@@ -18908,7 +18917,7 @@
       <c r="A257" s="3" t="s">
         <v>442</v>
       </c>
-      <c r="B257" s="34" t="s">
+      <c r="B257" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C257" s="6" t="s">
@@ -18952,7 +18961,7 @@
       <c r="A258" s="3" t="s">
         <v>444</v>
       </c>
-      <c r="B258" s="34" t="s">
+      <c r="B258" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C258" s="6" t="s">
@@ -18998,7 +19007,7 @@
       <c r="A259" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="B259" s="34" t="s">
+      <c r="B259" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C259" s="6" t="s">
@@ -19048,7 +19057,7 @@
       <c r="A260" s="3" t="s">
         <v>448</v>
       </c>
-      <c r="B260" s="34" t="s">
+      <c r="B260" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C260" s="6" t="s">
@@ -19098,7 +19107,7 @@
       <c r="A261" s="3" t="s">
         <v>450</v>
       </c>
-      <c r="B261" s="34" t="s">
+      <c r="B261" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C261" s="6" t="s">
@@ -19140,7 +19149,7 @@
       <c r="A262" s="3" t="s">
         <v>452</v>
       </c>
-      <c r="B262" s="34" t="s">
+      <c r="B262" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C262" s="6" t="s">
@@ -19182,7 +19191,7 @@
       <c r="A263" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="B263" s="34" t="s">
+      <c r="B263" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C263" s="6" t="s">
@@ -19224,7 +19233,7 @@
       <c r="A264" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="B264" s="34" t="s">
+      <c r="B264" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C264" s="6" t="s">
@@ -19266,7 +19275,7 @@
       <c r="A265" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="B265" s="34" t="s">
+      <c r="B265" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C265" s="6" t="s">
@@ -19312,7 +19321,7 @@
       <c r="A266" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="B266" s="34" t="s">
+      <c r="B266" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C266" s="6" t="s">
@@ -19358,7 +19367,7 @@
       <c r="A267" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="B267" s="34" t="s">
+      <c r="B267" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C267" s="6" t="s">
@@ -19404,7 +19413,7 @@
       <c r="A268" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="B268" s="34" t="s">
+      <c r="B268" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C268" s="6" t="s">
@@ -19446,7 +19455,7 @@
       <c r="A269" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="B269" s="34" t="s">
+      <c r="B269" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C269" s="6" t="s">
@@ -19486,7 +19495,7 @@
       <c r="A270" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="B270" s="34" t="s">
+      <c r="B270" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C270" s="6" t="s">
@@ -19526,7 +19535,7 @@
       <c r="A271" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="B271" s="34" t="s">
+      <c r="B271" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C271" s="6" t="s">
@@ -19570,7 +19579,7 @@
       <c r="A272" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="B272" s="34" t="s">
+      <c r="B272" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C272" s="6" t="s">
@@ -19610,7 +19619,7 @@
       <c r="A273" s="3" t="s">
         <v>465</v>
       </c>
-      <c r="B273" s="34" t="s">
+      <c r="B273" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C273" s="6" t="s">
@@ -19658,7 +19667,7 @@
       <c r="A274" s="3" t="s">
         <v>468</v>
       </c>
-      <c r="B274" s="34" t="s">
+      <c r="B274" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C274" s="6" t="s">
@@ -19698,7 +19707,7 @@
       <c r="A275" s="3" t="s">
         <v>469</v>
       </c>
-      <c r="B275" s="34" t="s">
+      <c r="B275" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C275" s="6" t="s">
@@ -19744,7 +19753,7 @@
       <c r="A276" s="3" t="s">
         <v>470</v>
       </c>
-      <c r="B276" s="34" t="s">
+      <c r="B276" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C276" s="6" t="s">
@@ -19790,7 +19799,7 @@
       <c r="A277" s="3" t="s">
         <v>472</v>
       </c>
-      <c r="B277" s="34" t="s">
+      <c r="B277" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C277" s="6" t="s">
@@ -19832,7 +19841,7 @@
       <c r="A278" s="3" t="s">
         <v>473</v>
       </c>
-      <c r="B278" s="34" t="s">
+      <c r="B278" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C278" s="6" t="s">
@@ -19872,7 +19881,7 @@
       <c r="A279" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="B279" s="34" t="s">
+      <c r="B279" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C279" s="6" t="s">
@@ -19920,7 +19929,7 @@
       <c r="A280" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="B280" s="34" t="s">
+      <c r="B280" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C280" s="6" t="s">
@@ -19976,7 +19985,7 @@
       <c r="A281" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="B281" s="34" t="s">
+      <c r="B281" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C281" s="6" t="s">
@@ -20032,7 +20041,7 @@
       <c r="A282" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="B282" s="34" t="s">
+      <c r="B282" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C282" s="6" t="s">
@@ -20086,7 +20095,7 @@
       <c r="A283" s="3" t="s">
         <v>479</v>
       </c>
-      <c r="B283" s="34" t="s">
+      <c r="B283" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C283" s="6" t="s">
@@ -20136,7 +20145,7 @@
       <c r="A284" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="B284" s="34" t="s">
+      <c r="B284" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C284" s="6" t="s">
@@ -20184,7 +20193,7 @@
       <c r="A285" s="3" t="s">
         <v>482</v>
       </c>
-      <c r="B285" s="34" t="s">
+      <c r="B285" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C285" s="6" t="s">
@@ -20226,7 +20235,7 @@
       <c r="A286" s="3" t="s">
         <v>483</v>
       </c>
-      <c r="B286" s="34" t="s">
+      <c r="B286" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C286" s="6" t="s">
@@ -20276,7 +20285,7 @@
       <c r="A287" s="3" t="s">
         <v>484</v>
       </c>
-      <c r="B287" s="34" t="s">
+      <c r="B287" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C287" s="6" t="s">
@@ -20334,7 +20343,7 @@
       <c r="A288" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="B288" s="34" t="s">
+      <c r="B288" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C288" s="6" t="s">
@@ -20380,7 +20389,7 @@
       <c r="A289" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="B289" s="34" t="s">
+      <c r="B289" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C289" s="6" t="s">
@@ -20422,7 +20431,7 @@
       <c r="A290" s="3" t="s">
         <v>488</v>
       </c>
-      <c r="B290" s="34" t="s">
+      <c r="B290" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C290" s="6" t="s">
@@ -20464,7 +20473,7 @@
       <c r="A291" s="3" t="s">
         <v>489</v>
       </c>
-      <c r="B291" s="34" t="s">
+      <c r="B291" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C291" s="6" t="s">
@@ -20504,7 +20513,7 @@
       <c r="A292" s="3" t="s">
         <v>490</v>
       </c>
-      <c r="B292" s="34" t="s">
+      <c r="B292" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C292" s="6" t="s">
@@ -20548,7 +20557,7 @@
       <c r="A293" s="3" t="s">
         <v>491</v>
       </c>
-      <c r="B293" s="34" t="s">
+      <c r="B293" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C293" s="6" t="s">
@@ -20590,7 +20599,7 @@
       <c r="A294" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="B294" s="34" t="s">
+      <c r="B294" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C294" s="6" t="s">
@@ -20632,7 +20641,7 @@
       <c r="A295" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="B295" s="34" t="s">
+      <c r="B295" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C295" s="6" t="s">
@@ -20676,7 +20685,7 @@
       <c r="A296" s="3" t="s">
         <v>495</v>
       </c>
-      <c r="B296" s="34" t="s">
+      <c r="B296" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C296" s="6" t="s">
@@ -20717,10 +20726,10 @@
       </c>
     </row>
     <row r="297" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A297" s="9" t="s">
+      <c r="A297" s="8" t="s">
         <v>496</v>
       </c>
-      <c r="B297" s="34" t="s">
+      <c r="B297" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C297" s="6" t="s">
@@ -20782,7 +20791,7 @@
       <c r="A298" s="3" t="s">
         <v>498</v>
       </c>
-      <c r="B298" s="34" t="s">
+      <c r="B298" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C298" s="6" t="s">
@@ -20834,7 +20843,7 @@
       <c r="A299" s="3" t="s">
         <v>500</v>
       </c>
-      <c r="B299" s="34" t="s">
+      <c r="B299" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C299" s="6" t="s">
@@ -20892,7 +20901,7 @@
       <c r="A300" s="3" t="s">
         <v>501</v>
       </c>
-      <c r="B300" s="34" t="s">
+      <c r="B300" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C300" s="6" t="s">
@@ -20934,7 +20943,7 @@
       <c r="A301" s="3" t="s">
         <v>502</v>
       </c>
-      <c r="B301" s="34" t="s">
+      <c r="B301" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C301" s="6" t="s">
@@ -20973,10 +20982,10 @@
       </c>
     </row>
     <row r="302" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A302" s="9" t="s">
+      <c r="A302" s="8" t="s">
         <v>503</v>
       </c>
-      <c r="B302" s="34" t="s">
+      <c r="B302" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C302" s="6" t="s">
@@ -21018,7 +21027,7 @@
       <c r="A303" s="3" t="s">
         <v>504</v>
       </c>
-      <c r="B303" s="34" t="s">
+      <c r="B303" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C303" s="6" t="s">
@@ -21057,10 +21066,10 @@
       </c>
     </row>
     <row r="304" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A304" s="9" t="s">
+      <c r="A304" s="8" t="s">
         <v>505</v>
       </c>
-      <c r="B304" s="34" t="s">
+      <c r="B304" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C304" s="6" t="s">
@@ -21110,7 +21119,7 @@
       <c r="A305" s="3" t="s">
         <v>507</v>
       </c>
-      <c r="B305" s="34" t="s">
+      <c r="B305" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C305" s="6" t="s">
@@ -21156,7 +21165,7 @@
       <c r="A306" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="B306" s="34" t="s">
+      <c r="B306" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C306" s="6" t="s">
@@ -21198,7 +21207,7 @@
       <c r="A307" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="B307" s="34" t="s">
+      <c r="B307" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C307" s="6" t="s">
@@ -21252,7 +21261,7 @@
       <c r="A308" s="3" t="s">
         <v>511</v>
       </c>
-      <c r="B308" s="34" t="s">
+      <c r="B308" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C308" s="6" t="s">
@@ -21294,7 +21303,7 @@
       <c r="A309" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="B309" s="34" t="s">
+      <c r="B309" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C309" s="6" t="s">
@@ -21336,7 +21345,7 @@
       <c r="A310" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="B310" s="34" t="s">
+      <c r="B310" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C310" s="6" t="s">
@@ -21396,7 +21405,7 @@
       <c r="A311" s="3" t="s">
         <v>514</v>
       </c>
-      <c r="B311" s="34" t="s">
+      <c r="B311" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C311" s="6" t="s">
@@ -21438,7 +21447,7 @@
       <c r="A312" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="B312" s="34" t="s">
+      <c r="B312" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C312" s="6" t="s">
@@ -21484,7 +21493,7 @@
       <c r="A313" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="B313" s="34" t="s">
+      <c r="B313" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C313" s="6" t="s">
@@ -21526,7 +21535,7 @@
       <c r="A314" s="3" t="s">
         <v>517</v>
       </c>
-      <c r="B314" s="34" t="s">
+      <c r="B314" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C314" s="6"/>
@@ -21566,7 +21575,7 @@
       <c r="A315" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="B315" s="34" t="s">
+      <c r="B315" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C315" s="6" t="s">
@@ -21612,7 +21621,7 @@
       <c r="A316" s="3" t="s">
         <v>520</v>
       </c>
-      <c r="B316" s="34" t="s">
+      <c r="B316" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C316" s="6" t="s">
@@ -21654,7 +21663,7 @@
       <c r="A317" s="3" t="s">
         <v>521</v>
       </c>
-      <c r="B317" s="34" t="s">
+      <c r="B317" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C317" s="6" t="s">
@@ -21700,7 +21709,7 @@
       <c r="A318" s="3" t="s">
         <v>523</v>
       </c>
-      <c r="B318" s="34" t="s">
+      <c r="B318" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C318" s="6" t="s">
@@ -21740,7 +21749,7 @@
       <c r="A319" s="3" t="s">
         <v>524</v>
       </c>
-      <c r="B319" s="34" t="s">
+      <c r="B319" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C319" s="6" t="s">
@@ -21786,7 +21795,7 @@
       <c r="A320" s="3" t="s">
         <v>526</v>
       </c>
-      <c r="B320" s="34" t="s">
+      <c r="B320" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C320" s="6" t="s">
@@ -21826,7 +21835,7 @@
       <c r="A321" s="3" t="s">
         <v>527</v>
       </c>
-      <c r="B321" s="34" t="s">
+      <c r="B321" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C321" s="6" t="s">
@@ -21876,7 +21885,7 @@
       <c r="A322" s="3" t="s">
         <v>528</v>
       </c>
-      <c r="B322" s="34" t="s">
+      <c r="B322" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C322" s="6" t="s">
@@ -21918,7 +21927,7 @@
       <c r="A323" s="3" t="s">
         <v>529</v>
       </c>
-      <c r="B323" s="34" t="s">
+      <c r="B323" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C323" s="6" t="s">
@@ -21964,7 +21973,7 @@
       <c r="A324" s="3" t="s">
         <v>530</v>
       </c>
-      <c r="B324" s="34" t="s">
+      <c r="B324" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C324" s="6" t="s">
@@ -22012,7 +22021,7 @@
       <c r="A325" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="B325" s="34" t="s">
+      <c r="B325" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C325" s="6" t="s">
@@ -22072,7 +22081,7 @@
       <c r="A326" s="3" t="s">
         <v>533</v>
       </c>
-      <c r="B326" s="34" t="s">
+      <c r="B326" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C326" s="6" t="s">
@@ -22114,7 +22123,7 @@
       <c r="A327" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="B327" s="34" t="s">
+      <c r="B327" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C327" s="6" t="s">
@@ -22156,7 +22165,7 @@
       <c r="A328" s="3" t="s">
         <v>535</v>
       </c>
-      <c r="B328" s="34" t="s">
+      <c r="B328" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C328" s="6" t="s">
@@ -22198,7 +22207,7 @@
       <c r="A329" s="3" t="s">
         <v>536</v>
       </c>
-      <c r="B329" s="34" t="s">
+      <c r="B329" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C329" s="6" t="s">
@@ -22244,7 +22253,7 @@
       <c r="A330" s="3" t="s">
         <v>538</v>
       </c>
-      <c r="B330" s="34" t="s">
+      <c r="B330" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C330" s="6" t="s">
@@ -22286,7 +22295,7 @@
       <c r="A331" s="3" t="s">
         <v>540</v>
       </c>
-      <c r="B331" s="34" t="s">
+      <c r="B331" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C331" s="6" t="s">
@@ -22328,7 +22337,7 @@
       <c r="A332" s="3" t="s">
         <v>541</v>
       </c>
-      <c r="B332" s="34" t="s">
+      <c r="B332" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C332" s="6" t="s">
@@ -22388,7 +22397,7 @@
       <c r="A333" s="3" t="s">
         <v>544</v>
       </c>
-      <c r="B333" s="34" t="s">
+      <c r="B333" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C333" s="6" t="s">
@@ -22430,7 +22439,7 @@
       <c r="A334" s="3" t="s">
         <v>545</v>
       </c>
-      <c r="B334" s="34" t="s">
+      <c r="B334" s="33" t="s">
         <v>609</v>
       </c>
       <c r="C334" s="6" t="s">
@@ -22469,52 +22478,52 @@
       </c>
     </row>
     <row r="335" spans="1:22" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A335" s="10" t="s">
+      <c r="A335" s="9" t="s">
         <v>546</v>
       </c>
-      <c r="B335" s="34" t="s">
+      <c r="B335" s="33" t="s">
         <v>609</v>
       </c>
-      <c r="C335" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D335" s="11"/>
-      <c r="E335" s="11"/>
-      <c r="F335" s="12"/>
-      <c r="G335" s="11">
+      <c r="C335" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D335" s="10"/>
+      <c r="E335" s="10"/>
+      <c r="F335" s="11"/>
+      <c r="G335" s="10">
         <v>1982</v>
       </c>
-      <c r="H335" s="11"/>
-      <c r="I335" s="11"/>
-      <c r="J335" s="12"/>
-      <c r="K335" s="12" t="s">
+      <c r="H335" s="10"/>
+      <c r="I335" s="10"/>
+      <c r="J335" s="11"/>
+      <c r="K335" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="L335" s="11"/>
-      <c r="M335" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="N335" s="11"/>
-      <c r="O335" s="12"/>
-      <c r="P335" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q335" s="11"/>
-      <c r="R335" s="11"/>
-      <c r="S335" s="11"/>
-      <c r="T335" s="12"/>
-      <c r="U335" s="12" t="s">
+      <c r="L335" s="10"/>
+      <c r="M335" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="N335" s="10"/>
+      <c r="O335" s="11"/>
+      <c r="P335" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q335" s="10"/>
+      <c r="R335" s="10"/>
+      <c r="S335" s="10"/>
+      <c r="T335" s="11"/>
+      <c r="U335" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="V335" s="11" t="s">
+      <c r="V335" s="10" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="336" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A336" s="9" t="s">
+      <c r="A336" s="8" t="s">
         <v>547</v>
       </c>
-      <c r="B336" s="35" t="s">
+      <c r="B336" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C336" s="4"/>
@@ -22561,10 +22570,10 @@
       </c>
     </row>
     <row r="337" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A337" s="9" t="s">
+      <c r="A337" s="8" t="s">
         <v>549</v>
       </c>
-      <c r="B337" s="35" t="s">
+      <c r="B337" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C337" s="4"/>
@@ -22607,10 +22616,10 @@
       </c>
     </row>
     <row r="338" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A338" s="9" t="s">
+      <c r="A338" s="8" t="s">
         <v>551</v>
       </c>
-      <c r="B338" s="35" t="s">
+      <c r="B338" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C338" s="4" t="s">
@@ -22657,10 +22666,10 @@
       </c>
     </row>
     <row r="339" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A339" s="9" t="s">
+      <c r="A339" s="8" t="s">
         <v>553</v>
       </c>
-      <c r="B339" s="35" t="s">
+      <c r="B339" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C339" s="4"/>
@@ -22699,10 +22708,10 @@
       </c>
     </row>
     <row r="340" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A340" s="9" t="s">
+      <c r="A340" s="8" t="s">
         <v>554</v>
       </c>
-      <c r="B340" s="35" t="s">
+      <c r="B340" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C340" s="4" t="s">
@@ -22741,10 +22750,10 @@
       </c>
     </row>
     <row r="341" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A341" s="9" t="s">
+      <c r="A341" s="8" t="s">
         <v>555</v>
       </c>
-      <c r="B341" s="35" t="s">
+      <c r="B341" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C341" s="4" t="s">
@@ -22783,10 +22792,10 @@
       </c>
     </row>
     <row r="342" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A342" s="9" t="s">
+      <c r="A342" s="8" t="s">
         <v>556</v>
       </c>
-      <c r="B342" s="35" t="s">
+      <c r="B342" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C342" s="4" t="s">
@@ -22831,10 +22840,10 @@
       </c>
     </row>
     <row r="343" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A343" s="9" t="s">
+      <c r="A343" s="8" t="s">
         <v>557</v>
       </c>
-      <c r="B343" s="35" t="s">
+      <c r="B343" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C343" s="4" t="s">
@@ -22873,10 +22882,10 @@
       </c>
     </row>
     <row r="344" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A344" s="9" t="s">
+      <c r="A344" s="8" t="s">
         <v>558</v>
       </c>
-      <c r="B344" s="35" t="s">
+      <c r="B344" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C344" s="4"/>
@@ -22915,10 +22924,10 @@
       </c>
     </row>
     <row r="345" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A345" s="9" t="s">
+      <c r="A345" s="8" t="s">
         <v>559</v>
       </c>
-      <c r="B345" s="35" t="s">
+      <c r="B345" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C345" s="4" t="s">
@@ -22967,10 +22976,10 @@
       </c>
     </row>
     <row r="346" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A346" s="9" t="s">
+      <c r="A346" s="8" t="s">
         <v>562</v>
       </c>
-      <c r="B346" s="35" t="s">
+      <c r="B346" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C346" s="4"/>
@@ -23009,10 +23018,10 @@
       </c>
     </row>
     <row r="347" spans="1:22" ht="51" x14ac:dyDescent="0.25">
-      <c r="A347" s="9" t="s">
+      <c r="A347" s="8" t="s">
         <v>564</v>
       </c>
-      <c r="B347" s="35" t="s">
+      <c r="B347" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C347" s="4" t="s">
@@ -23053,10 +23062,10 @@
       </c>
     </row>
     <row r="348" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A348" s="9" t="s">
+      <c r="A348" s="8" t="s">
         <v>565</v>
       </c>
-      <c r="B348" s="35" t="s">
+      <c r="B348" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C348" s="4" t="s">
@@ -23099,10 +23108,10 @@
       </c>
     </row>
     <row r="349" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A349" s="9" t="s">
+      <c r="A349" s="8" t="s">
         <v>566</v>
       </c>
-      <c r="B349" s="35" t="s">
+      <c r="B349" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C349" s="4" t="s">
@@ -23151,10 +23160,10 @@
       </c>
     </row>
     <row r="350" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A350" s="9" t="s">
+      <c r="A350" s="8" t="s">
         <v>568</v>
       </c>
-      <c r="B350" s="35" t="s">
+      <c r="B350" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C350" s="4"/>
@@ -23189,10 +23198,10 @@
       </c>
     </row>
     <row r="351" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A351" s="9" t="s">
+      <c r="A351" s="8" t="s">
         <v>569</v>
       </c>
-      <c r="B351" s="35" t="s">
+      <c r="B351" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C351" s="4" t="s">
@@ -23245,10 +23254,10 @@
       </c>
     </row>
     <row r="352" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A352" s="9" t="s">
+      <c r="A352" s="8" t="s">
         <v>571</v>
       </c>
-      <c r="B352" s="35" t="s">
+      <c r="B352" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C352" s="4" t="s">
@@ -23301,10 +23310,10 @@
       </c>
     </row>
     <row r="353" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A353" s="9" t="s">
+      <c r="A353" s="8" t="s">
         <v>573</v>
       </c>
-      <c r="B353" s="35" t="s">
+      <c r="B353" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C353" s="4" t="s">
@@ -23357,10 +23366,10 @@
       </c>
     </row>
     <row r="354" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A354" s="9" t="s">
+      <c r="A354" s="8" t="s">
         <v>575</v>
       </c>
-      <c r="B354" s="35" t="s">
+      <c r="B354" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C354" s="4" t="s">
@@ -23415,10 +23424,10 @@
       </c>
     </row>
     <row r="355" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A355" s="9" t="s">
+      <c r="A355" s="8" t="s">
         <v>577</v>
       </c>
-      <c r="B355" s="35" t="s">
+      <c r="B355" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C355" s="4" t="s">
@@ -23477,10 +23486,10 @@
       </c>
     </row>
     <row r="356" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A356" s="9" t="s">
+      <c r="A356" s="8" t="s">
         <v>578</v>
       </c>
-      <c r="B356" s="35" t="s">
+      <c r="B356" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C356" s="4" t="s">
@@ -23521,10 +23530,10 @@
       </c>
     </row>
     <row r="357" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A357" s="9" t="s">
+      <c r="A357" s="8" t="s">
         <v>579</v>
       </c>
-      <c r="B357" s="35" t="s">
+      <c r="B357" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C357" s="4" t="s">
@@ -23577,10 +23586,10 @@
       </c>
     </row>
     <row r="358" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A358" s="9" t="s">
+      <c r="A358" s="8" t="s">
         <v>581</v>
       </c>
-      <c r="B358" s="35" t="s">
+      <c r="B358" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C358" s="4" t="s">
@@ -23625,10 +23634,10 @@
       </c>
     </row>
     <row r="359" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A359" s="9" t="s">
+      <c r="A359" s="8" t="s">
         <v>583</v>
       </c>
-      <c r="B359" s="35" t="s">
+      <c r="B359" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C359" s="4"/>
@@ -23671,10 +23680,10 @@
       </c>
     </row>
     <row r="360" spans="1:22" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A360" s="9" t="s">
+      <c r="A360" s="8" t="s">
         <v>584</v>
       </c>
-      <c r="B360" s="35" t="s">
+      <c r="B360" s="34" t="s">
         <v>610</v>
       </c>
       <c r="C360" s="4" t="s">

</xml_diff>